<commit_message>
update from dell msysgit
</commit_message>
<xml_diff>
--- a/anhei2/sell.xlsx
+++ b/anhei2/sell.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="sell" sheetId="1" r:id="rId1"/>
@@ -429,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -456,15 +456,24 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -527,7 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>